<commit_message>
presales changes data capturing
</commit_message>
<xml_diff>
--- a/src/assets/tamplate/BOQ_sample_template.xlsx
+++ b/src/assets/tamplate/BOQ_sample_template.xlsx
@@ -5,15 +5,15 @@
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\D\LIVE PROJECTS\GEPDEC Infra Software Development\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\D\LIVE PROJECTS\GEPDEC Infra Software Development\GEPDEC INFRA APP\APP\src\assets\tamplate\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{33415354-0A63-4F78-AA30-0A6166850632}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{84C510BB-C43D-4530-8E4C-ECE5298C5CA8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{B7C91633-A693-480F-A3C1-18EBEC19EE60}"/>
   </bookViews>
   <sheets>
-    <sheet name="BOQ Sample Template" sheetId="3" r:id="rId1"/>
+    <sheet name="BOQ_sample_template" sheetId="3" r:id="rId1"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -36,68 +36,12 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="26" uniqueCount="17">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6" uniqueCount="6">
   <si>
     <t>S No.</t>
   </si>
   <si>
-    <t>Power Transformers</t>
-  </si>
-  <si>
-    <t>220/132kV, 160 MVA</t>
-  </si>
-  <si>
-    <t>Heat run test</t>
-  </si>
-  <si>
-    <t>Impulse test</t>
-  </si>
-  <si>
-    <t>220/33kV, 60 MVA</t>
-  </si>
-  <si>
-    <t>245kV GIS Equipment</t>
-  </si>
-  <si>
-    <r>
-      <t xml:space="preserve">245kV, 1600A, 40 kA for 1 sec, SF6 gas insulated bay module each comprising of SF6 gas insulated circuit breaker, current transformer, bus-bar disconnectors with common grounding switch, disconnector with safety grounding switchfes), local control cubicle, SF6 gas monitoring system,double bus bar for complete bay, gas insulated terminal connection for connecting XLPE Cable) with GIS etc. to complete </t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="12"/>
-        <rFont val="Times New Roman"/>
-        <family val="1"/>
-      </rPr>
-      <t>Transformer Bay Module.132 kv transformer 160 mva</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <t xml:space="preserve">245kV, 1600 A, 40 kA for 1 sec, SF6 gas insulated bay module each comprising of SF6 gas insulated circuit breaker, current transformer, bus-bar disconnectors with common grounding switch, disconnector with safety grounding switch(es), local control cubicle, SF6 gas monitoring system,double bus bar for complete bay, gas insulated terminal connection for connecting XLPE Cable) with GIS etc, to complete </t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="12"/>
-        <rFont val="Times New Roman"/>
-        <family val="1"/>
-      </rPr>
-      <t>Transformer Bay Module. 
-60 mva transformer</t>
-    </r>
-  </si>
-  <si>
     <t>Unit</t>
-  </si>
-  <si>
-    <t>No</t>
-  </si>
-  <si>
-    <t>Set.</t>
-  </si>
-  <si>
-    <t>set</t>
   </si>
   <si>
     <t>Qty</t>
@@ -116,24 +60,13 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Aptos Narrow"/>
       <family val="2"/>
       <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="12"/>
-      <name val="Times New Roman"/>
-      <family val="1"/>
-    </font>
-    <font>
-      <sz val="12"/>
-      <name val="Times New Roman"/>
-      <family val="1"/>
     </font>
     <font>
       <b/>
@@ -144,7 +77,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="4">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -153,18 +86,12 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="0"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor rgb="FF0070C0"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
   </fills>
-  <borders count="2">
+  <borders count="1">
     <border>
       <left/>
       <right/>
@@ -172,41 +99,13 @@
       <bottom/>
       <diagonal/>
     </border>
-    <border>
-      <left style="thin">
-        <color indexed="64"/>
-      </left>
-      <right style="thin">
-        <color indexed="64"/>
-      </right>
-      <top style="thin">
-        <color indexed="64"/>
-      </top>
-      <bottom style="thin">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -541,10 +440,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D9F695BE-98C0-413B-BA5B-A189F48CD178}">
-  <dimension ref="A1:F12"/>
+  <dimension ref="A1:F1"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H10" sqref="H10"/>
+      <selection activeCell="G7" sqref="G7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -555,203 +454,26 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:6" ht="22.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="6" t="s">
+      <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="6" t="s">
-        <v>16</v>
-      </c>
-      <c r="C1" s="6" t="s">
-        <v>15</v>
-      </c>
-      <c r="D1" s="6" t="s">
-        <v>9</v>
-      </c>
-      <c r="E1" s="6" t="s">
-        <v>13</v>
-      </c>
-      <c r="F1" s="6" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="2" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A2" s="1">
+      <c r="B1" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="D1" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="1"/>
-      <c r="C2" s="2" t="s">
-        <v>1</v>
-      </c>
-      <c r="D2" s="3" t="s">
-        <v>10</v>
-      </c>
-      <c r="E2" s="5">
-        <v>5</v>
-      </c>
-      <c r="F2" s="5"/>
-    </row>
-    <row r="3" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A3" s="3">
-        <v>1.1000000000000001</v>
-      </c>
-      <c r="B3" s="3"/>
-      <c r="C3" s="4" t="s">
+      <c r="E1" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="D3" s="3" t="s">
-        <v>10</v>
-      </c>
-      <c r="E3" s="5">
-        <v>5</v>
-      </c>
-      <c r="F3" s="5"/>
-    </row>
-    <row r="4" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A4" s="3">
-        <v>1.2</v>
-      </c>
-      <c r="B4" s="3"/>
-      <c r="C4" s="4" t="s">
+      <c r="F1" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="D4" s="3" t="s">
-        <v>10</v>
-      </c>
-      <c r="E4" s="5">
-        <v>7</v>
-      </c>
-      <c r="F4" s="5"/>
-    </row>
-    <row r="5" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A5" s="3">
-        <v>1.3</v>
-      </c>
-      <c r="B5" s="3"/>
-      <c r="C5" s="4" t="s">
-        <v>4</v>
-      </c>
-      <c r="D5" s="3" t="s">
-        <v>10</v>
-      </c>
-      <c r="E5" s="5">
-        <v>9</v>
-      </c>
-      <c r="F5" s="5"/>
-    </row>
-    <row r="6" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A6" s="1">
-        <v>2</v>
-      </c>
-      <c r="B6" s="1"/>
-      <c r="C6" s="2" t="s">
-        <v>1</v>
-      </c>
-      <c r="D6" s="3"/>
-      <c r="E6" s="5">
-        <v>7</v>
-      </c>
-      <c r="F6" s="5"/>
-    </row>
-    <row r="7" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A7" s="3">
-        <v>2.1</v>
-      </c>
-      <c r="B7" s="3"/>
-      <c r="C7" s="4" t="s">
-        <v>5</v>
-      </c>
-      <c r="D7" s="3" t="s">
-        <v>10</v>
-      </c>
-      <c r="E7" s="5">
-        <v>6</v>
-      </c>
-      <c r="F7" s="5"/>
-    </row>
-    <row r="8" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A8" s="3">
-        <v>2.2000000000000002</v>
-      </c>
-      <c r="B8" s="3"/>
-      <c r="C8" s="4" t="s">
-        <v>3</v>
-      </c>
-      <c r="D8" s="3" t="s">
-        <v>10</v>
-      </c>
-      <c r="E8" s="5">
-        <v>2</v>
-      </c>
-      <c r="F8" s="5"/>
-    </row>
-    <row r="9" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A9" s="3">
-        <v>2.2999999999999998</v>
-      </c>
-      <c r="B9" s="3"/>
-      <c r="C9" s="4" t="s">
-        <v>4</v>
-      </c>
-      <c r="D9" s="3" t="s">
-        <v>10</v>
-      </c>
-      <c r="E9" s="5">
-        <v>4</v>
-      </c>
-      <c r="F9" s="5"/>
-    </row>
-    <row r="10" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A10" s="1">
-        <v>3</v>
-      </c>
-      <c r="B10" s="1"/>
-      <c r="C10" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="D10" s="3"/>
-      <c r="E10" s="5">
-        <v>6</v>
-      </c>
-      <c r="F10" s="5"/>
-    </row>
-    <row r="11" spans="1:6" ht="168" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A11" s="3">
-        <v>3.1</v>
-      </c>
-      <c r="B11" s="3"/>
-      <c r="C11" s="4" t="s">
-        <v>7</v>
-      </c>
-      <c r="D11" s="3" t="s">
-        <v>11</v>
-      </c>
-      <c r="E11" s="5">
-        <v>7</v>
-      </c>
-      <c r="F11" s="5"/>
-    </row>
-    <row r="12" spans="1:6" ht="146.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A12" s="3">
-        <v>3.2</v>
-      </c>
-      <c r="B12" s="3"/>
-      <c r="C12" s="4" t="s">
-        <v>8</v>
-      </c>
-      <c r="D12" s="3" t="s">
-        <v>12</v>
-      </c>
-      <c r="E12" s="5">
-        <v>8</v>
-      </c>
-      <c r="F12" s="5"/>
     </row>
   </sheetData>
-  <dataValidations count="1">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="F2:F12" xr:uid="{9C0909DA-EA11-42F8-A286-1826E7B42420}">
-      <formula1>"Billable,Non-Billable"</formula1>
-    </dataValidation>
-  </dataValidations>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>